<commit_message>
Some LanguageResource cleanup: updated some docs, removed some unneeded GAPP files, small additions to test data, fixed missing dependency in build.xml
</commit_message>
<xml_diff>
--- a/LanguageResources/docs/OpenSextant Entities.xlsx
+++ b/LanguageResources/docs/OpenSextant Entities.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Hierarchy Roots" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$I$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Schema!$A$1:$F$118</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="215">
   <si>
     <t>Crime</t>
   </si>
@@ -620,12 +620,6 @@
     <t>PLACE</t>
   </si>
   <si>
-    <t>GeneralPurpose Lite</t>
-  </si>
-  <si>
-    <t>General Purpose Full</t>
-  </si>
-  <si>
     <t>Hierarchy root</t>
   </si>
   <si>
@@ -668,10 +662,7 @@
     <t>Attribute.weight</t>
   </si>
   <si>
-    <t>Geocoords Only</t>
-  </si>
-  <si>
-    <t>Basic</t>
+    <t>General Purpose</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:F118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,15 +1012,12 @@
     <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>154</v>
       </c>
@@ -1040,375 +1028,366 @@
         <v>191</v>
       </c>
       <c r="D1" t="s">
-        <v>216</v>
+        <v>163</v>
       </c>
       <c r="E1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" t="s">
-        <v>200</v>
-      </c>
-      <c r="H1" t="s">
-        <v>201</v>
-      </c>
-      <c r="I1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
-        <v>186</v>
-      </c>
-      <c r="I2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="H3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
-        <v>186</v>
-      </c>
-      <c r="I4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="H5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>186</v>
+      </c>
+      <c r="F5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" t="s">
-        <v>186</v>
-      </c>
-      <c r="I6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>186</v>
+      </c>
+      <c r="F6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="H7" t="s">
-        <v>186</v>
-      </c>
-      <c r="I7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="H8" t="s">
-        <v>186</v>
-      </c>
-      <c r="I8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="H9" t="s">
-        <v>186</v>
-      </c>
-      <c r="I9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="H10" t="s">
-        <v>186</v>
-      </c>
-      <c r="I10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="H11" t="s">
-        <v>186</v>
-      </c>
-      <c r="I11" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" t="s">
-        <v>186</v>
-      </c>
-      <c r="I12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>215</v>
-      </c>
-      <c r="H13" t="s">
-        <v>186</v>
-      </c>
-      <c r="I13" t="s">
+        <v>213</v>
+      </c>
+      <c r="E13" t="s">
+        <v>186</v>
+      </c>
+      <c r="F13" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
-      </c>
-      <c r="H14" t="s">
-        <v>186</v>
-      </c>
-      <c r="I14" t="s">
+        <v>211</v>
+      </c>
+      <c r="E14" t="s">
+        <v>186</v>
+      </c>
+      <c r="F14" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
-      </c>
-      <c r="H15" t="s">
-        <v>186</v>
-      </c>
-      <c r="I15" t="s">
+        <v>209</v>
+      </c>
+      <c r="E15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="H16" t="s">
-        <v>186</v>
-      </c>
-      <c r="I16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
       </c>
-      <c r="H17" t="s">
-        <v>186</v>
-      </c>
-      <c r="I17" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
-      <c r="H18" t="s">
-        <v>186</v>
-      </c>
-      <c r="I18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>186</v>
+      </c>
+      <c r="F18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="H19" t="s">
-        <v>186</v>
-      </c>
-      <c r="I19" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>186</v>
+      </c>
+      <c r="F19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20" t="s">
         <v>28</v>
       </c>
-      <c r="H20" t="s">
-        <v>186</v>
-      </c>
-      <c r="I20" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>186</v>
+      </c>
+      <c r="F20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="H21" t="s">
-        <v>186</v>
-      </c>
-      <c r="I21" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>186</v>
+      </c>
+      <c r="F21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="H22" t="s">
-        <v>186</v>
-      </c>
-      <c r="I22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>186</v>
+      </c>
+      <c r="F22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>31</v>
       </c>
-      <c r="H23" t="s">
-        <v>186</v>
-      </c>
-      <c r="I23" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>186</v>
+      </c>
+      <c r="F23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="H24" t="s">
-        <v>186</v>
-      </c>
-      <c r="I24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>186</v>
+      </c>
+      <c r="F24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>33</v>
       </c>
-      <c r="H25" t="s">
-        <v>186</v>
-      </c>
-      <c r="I25" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>186</v>
+      </c>
+      <c r="F25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="H26" t="s">
-        <v>186</v>
-      </c>
-      <c r="I26" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>186</v>
+      </c>
+      <c r="F26" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>159</v>
       </c>
@@ -1425,19 +1404,10 @@
         <v>186</v>
       </c>
       <c r="F27" t="s">
-        <v>186</v>
-      </c>
-      <c r="G27" t="s">
-        <v>186</v>
-      </c>
-      <c r="H27" t="s">
-        <v>186</v>
-      </c>
-      <c r="I27" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>199</v>
       </c>
@@ -1447,118 +1417,115 @@
       <c r="C28" t="s">
         <v>181</v>
       </c>
+      <c r="D28" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" t="s">
+        <v>186</v>
+      </c>
       <c r="F28" t="s">
-        <v>186</v>
-      </c>
-      <c r="G28" t="s">
-        <v>186</v>
-      </c>
-      <c r="H28" t="s">
-        <v>186</v>
-      </c>
-      <c r="I28" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
       <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="H29" t="s">
-        <v>186</v>
-      </c>
-      <c r="I29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="H30" t="s">
-        <v>186</v>
-      </c>
-      <c r="I30" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>186</v>
+      </c>
+      <c r="F30" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>38</v>
       </c>
-      <c r="H31" t="s">
-        <v>186</v>
-      </c>
-      <c r="I31" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>186</v>
+      </c>
+      <c r="F31" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>40</v>
       </c>
-      <c r="H32" t="s">
-        <v>186</v>
-      </c>
-      <c r="I32" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
       </c>
-      <c r="H33" t="s">
-        <v>186</v>
-      </c>
-      <c r="I33" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
       <c r="B34" t="s">
         <v>44</v>
       </c>
-      <c r="H34" t="s">
-        <v>186</v>
-      </c>
-      <c r="I34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>186</v>
+      </c>
+      <c r="F34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>165</v>
       </c>
       <c r="B35" t="s">
         <v>164</v>
       </c>
-      <c r="H35" t="s">
-        <v>186</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="E35" t="s">
+        <v>186</v>
+      </c>
+      <c r="F35" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>189</v>
       </c>
@@ -1568,17 +1535,11 @@
       <c r="E36" t="s">
         <v>186</v>
       </c>
-      <c r="G36" t="s">
-        <v>186</v>
-      </c>
-      <c r="H36" t="s">
-        <v>186</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="F36" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>184</v>
       </c>
@@ -1588,17 +1549,11 @@
       <c r="E37" t="s">
         <v>186</v>
       </c>
-      <c r="G37" t="s">
-        <v>186</v>
-      </c>
-      <c r="H37" t="s">
-        <v>186</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="F37" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>183</v>
       </c>
@@ -1608,241 +1563,235 @@
       <c r="E38" t="s">
         <v>186</v>
       </c>
-      <c r="G38" t="s">
-        <v>186</v>
-      </c>
-      <c r="H38" t="s">
-        <v>186</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="F38" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
       <c r="B39" t="s">
         <v>46</v>
       </c>
-      <c r="H39" t="s">
-        <v>186</v>
-      </c>
-      <c r="I39" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>47</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
       </c>
-      <c r="H40" t="s">
-        <v>186</v>
-      </c>
-      <c r="I40" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>186</v>
+      </c>
+      <c r="F40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>170</v>
       </c>
       <c r="B41" t="s">
         <v>169</v>
       </c>
-      <c r="H41" t="s">
-        <v>186</v>
-      </c>
-      <c r="I41" t="s">
+      <c r="E41" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>176</v>
       </c>
       <c r="B42" t="s">
         <v>175</v>
       </c>
-      <c r="H42" t="s">
-        <v>186</v>
-      </c>
-      <c r="I42" t="s">
+      <c r="E42" t="s">
+        <v>186</v>
+      </c>
+      <c r="F42" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>172</v>
       </c>
       <c r="B43" t="s">
         <v>171</v>
       </c>
-      <c r="H43" t="s">
-        <v>186</v>
-      </c>
-      <c r="I43" t="s">
+      <c r="E43" t="s">
+        <v>186</v>
+      </c>
+      <c r="F43" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>174</v>
       </c>
       <c r="B44" t="s">
         <v>173</v>
       </c>
-      <c r="H44" t="s">
-        <v>186</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="E44" t="s">
+        <v>186</v>
+      </c>
+      <c r="F44" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>73</v>
       </c>
       <c r="B45" t="s">
         <v>73</v>
       </c>
-      <c r="H45" t="s">
-        <v>186</v>
-      </c>
-      <c r="I45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>186</v>
+      </c>
+      <c r="F45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
       <c r="B46" t="s">
         <v>54</v>
       </c>
-      <c r="H46" t="s">
-        <v>186</v>
-      </c>
-      <c r="I46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
+        <v>186</v>
+      </c>
+      <c r="F46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>57</v>
       </c>
       <c r="B47" t="s">
         <v>58</v>
       </c>
-      <c r="H47" t="s">
-        <v>186</v>
-      </c>
-      <c r="I47" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>186</v>
+      </c>
+      <c r="F47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>61</v>
       </c>
       <c r="B48" t="s">
         <v>62</v>
       </c>
-      <c r="H48" t="s">
-        <v>186</v>
-      </c>
-      <c r="I48" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>186</v>
+      </c>
+      <c r="F48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>63</v>
       </c>
       <c r="B49" t="s">
         <v>64</v>
       </c>
-      <c r="H49" t="s">
-        <v>186</v>
-      </c>
-      <c r="I49" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>65</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
       </c>
-      <c r="H50" t="s">
-        <v>186</v>
-      </c>
-      <c r="I50" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>186</v>
+      </c>
+      <c r="F50" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>67</v>
       </c>
       <c r="B51" t="s">
         <v>68</v>
       </c>
-      <c r="H51" t="s">
-        <v>186</v>
-      </c>
-      <c r="I51" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
+        <v>186</v>
+      </c>
+      <c r="F51" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>59</v>
       </c>
       <c r="B52" t="s">
         <v>60</v>
       </c>
-      <c r="H52" t="s">
-        <v>186</v>
-      </c>
-      <c r="I52" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
+        <v>186</v>
+      </c>
+      <c r="F52" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>80</v>
       </c>
       <c r="B53" t="s">
         <v>81</v>
       </c>
-      <c r="H53" t="s">
-        <v>186</v>
-      </c>
-      <c r="I53" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>186</v>
+      </c>
+      <c r="F53" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>195</v>
       </c>
       <c r="B54" t="s">
         <v>196</v>
       </c>
-      <c r="H54" t="s">
-        <v>186</v>
-      </c>
-      <c r="I54" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>186</v>
+      </c>
+      <c r="F54" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -1852,773 +1801,767 @@
       <c r="E55" t="s">
         <v>186</v>
       </c>
-      <c r="G55" t="s">
-        <v>186</v>
-      </c>
-      <c r="H55" t="s">
-        <v>186</v>
-      </c>
-      <c r="I55" t="s">
+      <c r="F55" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>74</v>
       </c>
       <c r="B56" t="s">
         <v>75</v>
       </c>
-      <c r="H56" t="s">
-        <v>186</v>
-      </c>
-      <c r="I56" t="s">
+      <c r="E56" t="s">
+        <v>186</v>
+      </c>
+      <c r="F56" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
       <c r="B57" t="s">
         <v>70</v>
       </c>
-      <c r="H57" t="s">
-        <v>186</v>
-      </c>
-      <c r="I57" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>186</v>
+      </c>
+      <c r="F57" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>82</v>
       </c>
       <c r="B58" t="s">
         <v>83</v>
       </c>
-      <c r="H58" t="s">
-        <v>186</v>
-      </c>
-      <c r="I58" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
+        <v>186</v>
+      </c>
+      <c r="F58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>49</v>
       </c>
       <c r="B59" t="s">
         <v>50</v>
       </c>
-      <c r="H59" t="s">
-        <v>186</v>
-      </c>
-      <c r="I59" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>49</v>
       </c>
       <c r="B60" t="s">
         <v>51</v>
       </c>
-      <c r="H60" t="s">
-        <v>186</v>
-      </c>
-      <c r="I60" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
+        <v>186</v>
+      </c>
+      <c r="F60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>49</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
       </c>
-      <c r="H61" t="s">
-        <v>186</v>
-      </c>
-      <c r="I61" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
+        <v>186</v>
+      </c>
+      <c r="F61" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>71</v>
       </c>
       <c r="B62" t="s">
         <v>72</v>
       </c>
-      <c r="H62" t="s">
-        <v>186</v>
-      </c>
-      <c r="I62" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
+        <v>186</v>
+      </c>
+      <c r="F62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B63" t="s">
-        <v>204</v>
-      </c>
-      <c r="H63" t="s">
-        <v>186</v>
-      </c>
-      <c r="I63" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+      <c r="E63" t="s">
+        <v>186</v>
+      </c>
+      <c r="F63" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>55</v>
       </c>
       <c r="B64" t="s">
         <v>56</v>
       </c>
-      <c r="H64" t="s">
-        <v>186</v>
-      </c>
-      <c r="I64" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
+        <v>186</v>
+      </c>
+      <c r="F64" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>205</v>
-      </c>
-      <c r="H65" t="s">
-        <v>186</v>
-      </c>
-      <c r="I65" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="E65" t="s">
+        <v>186</v>
+      </c>
+      <c r="F65" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
       <c r="B66" t="s">
         <v>77</v>
       </c>
-      <c r="H66" t="s">
-        <v>186</v>
-      </c>
-      <c r="I66" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
+        <v>186</v>
+      </c>
+      <c r="F66" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B67" t="s">
-        <v>207</v>
-      </c>
-      <c r="H67" t="s">
-        <v>186</v>
-      </c>
-      <c r="I67" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>205</v>
+      </c>
+      <c r="E67" t="s">
+        <v>186</v>
+      </c>
+      <c r="F67" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>78</v>
       </c>
       <c r="B68" t="s">
         <v>79</v>
       </c>
-      <c r="H68" t="s">
-        <v>186</v>
-      </c>
-      <c r="I68" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
+        <v>186</v>
+      </c>
+      <c r="F68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>90</v>
       </c>
       <c r="B69" t="s">
         <v>91</v>
       </c>
-      <c r="H69" t="s">
-        <v>186</v>
-      </c>
-      <c r="I69" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
+        <v>186</v>
+      </c>
+      <c r="F69" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
       <c r="B70" t="s">
         <v>85</v>
       </c>
-      <c r="H70" t="s">
-        <v>186</v>
-      </c>
-      <c r="I70" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
+        <v>186</v>
+      </c>
+      <c r="F70" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>86</v>
       </c>
       <c r="B71" t="s">
         <v>87</v>
       </c>
-      <c r="H71" t="s">
-        <v>186</v>
-      </c>
-      <c r="I71" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>186</v>
+      </c>
+      <c r="F71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>88</v>
       </c>
       <c r="B72" t="s">
         <v>89</v>
       </c>
-      <c r="H72" t="s">
-        <v>186</v>
-      </c>
-      <c r="I72" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
+        <v>186</v>
+      </c>
+      <c r="F72" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>92</v>
       </c>
       <c r="B73" t="s">
         <v>92</v>
       </c>
-      <c r="H73" t="s">
-        <v>186</v>
-      </c>
-      <c r="I73" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
+        <v>186</v>
+      </c>
+      <c r="F73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>99</v>
       </c>
       <c r="B74" t="s">
         <v>93</v>
       </c>
-      <c r="H74" t="s">
-        <v>186</v>
-      </c>
-      <c r="I74" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
+        <v>186</v>
+      </c>
+      <c r="F74" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>100</v>
       </c>
       <c r="B75" t="s">
         <v>101</v>
       </c>
-      <c r="H75" t="s">
-        <v>186</v>
-      </c>
-      <c r="I75" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
+        <v>186</v>
+      </c>
+      <c r="F75" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>92</v>
       </c>
       <c r="B76" t="s">
         <v>94</v>
       </c>
-      <c r="H76" t="s">
-        <v>186</v>
-      </c>
-      <c r="I76" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
+        <v>186</v>
+      </c>
+      <c r="F76" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>104</v>
       </c>
       <c r="B77" t="s">
         <v>105</v>
       </c>
-      <c r="H77" t="s">
-        <v>186</v>
-      </c>
-      <c r="I77" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
+        <v>186</v>
+      </c>
+      <c r="F77" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>92</v>
       </c>
       <c r="B78" t="s">
         <v>108</v>
       </c>
-      <c r="H78" t="s">
-        <v>186</v>
-      </c>
-      <c r="I78" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
+        <v>186</v>
+      </c>
+      <c r="F78" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>92</v>
       </c>
       <c r="B79" t="s">
         <v>95</v>
       </c>
-      <c r="H79" t="s">
-        <v>186</v>
-      </c>
-      <c r="I79" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>186</v>
+      </c>
+      <c r="F79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>92</v>
       </c>
       <c r="B80" t="s">
         <v>102</v>
       </c>
-      <c r="H80" t="s">
-        <v>186</v>
-      </c>
-      <c r="I80" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>186</v>
+      </c>
+      <c r="F80" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>197</v>
       </c>
       <c r="B81" t="s">
         <v>198</v>
       </c>
-      <c r="H81" t="s">
-        <v>186</v>
-      </c>
-      <c r="I81" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>186</v>
+      </c>
+      <c r="F81" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>92</v>
       </c>
       <c r="B82" t="s">
         <v>103</v>
       </c>
-      <c r="H82" t="s">
-        <v>186</v>
-      </c>
-      <c r="I82" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>186</v>
+      </c>
+      <c r="F82" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>92</v>
       </c>
       <c r="B83" t="s">
         <v>96</v>
       </c>
-      <c r="H83" t="s">
-        <v>186</v>
-      </c>
-      <c r="I83" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>186</v>
+      </c>
+      <c r="F83" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>106</v>
       </c>
       <c r="B84" t="s">
         <v>107</v>
       </c>
-      <c r="H84" t="s">
-        <v>186</v>
-      </c>
-      <c r="I84" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>186</v>
+      </c>
+      <c r="F84" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>97</v>
       </c>
       <c r="B85" t="s">
         <v>98</v>
       </c>
-      <c r="H85" t="s">
-        <v>186</v>
-      </c>
-      <c r="I85" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>186</v>
+      </c>
+      <c r="F85" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>125</v>
       </c>
       <c r="B86" t="s">
         <v>125</v>
       </c>
-      <c r="H86" t="s">
-        <v>186</v>
-      </c>
-      <c r="I86" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>186</v>
+      </c>
+      <c r="F86" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>113</v>
       </c>
       <c r="B87" t="s">
         <v>114</v>
       </c>
-      <c r="H87" t="s">
-        <v>186</v>
-      </c>
-      <c r="I87" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>186</v>
+      </c>
+      <c r="F87" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>113</v>
       </c>
       <c r="B88" t="s">
         <v>115</v>
       </c>
-      <c r="H88" t="s">
-        <v>186</v>
-      </c>
-      <c r="I88" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>186</v>
+      </c>
+      <c r="F88" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>113</v>
       </c>
       <c r="B89" t="s">
         <v>116</v>
       </c>
-      <c r="H89" t="s">
-        <v>186</v>
-      </c>
-      <c r="I89" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>186</v>
+      </c>
+      <c r="F89" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>109</v>
       </c>
       <c r="B90" t="s">
         <v>110</v>
       </c>
-      <c r="H90" t="s">
-        <v>186</v>
-      </c>
-      <c r="I90" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>186</v>
+      </c>
+      <c r="F90" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>117</v>
       </c>
       <c r="B91" t="s">
         <v>118</v>
       </c>
-      <c r="H91" t="s">
-        <v>186</v>
-      </c>
-      <c r="I91" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>186</v>
+      </c>
+      <c r="F91" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>119</v>
       </c>
       <c r="B92" t="s">
         <v>120</v>
       </c>
-      <c r="H92" t="s">
-        <v>186</v>
-      </c>
-      <c r="I92" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>186</v>
+      </c>
+      <c r="F92" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>111</v>
       </c>
       <c r="B93" t="s">
         <v>112</v>
       </c>
-      <c r="H93" t="s">
-        <v>186</v>
-      </c>
-      <c r="I93" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>186</v>
+      </c>
+      <c r="F93" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>121</v>
       </c>
       <c r="B94" t="s">
         <v>122</v>
       </c>
-      <c r="H94" t="s">
-        <v>186</v>
-      </c>
-      <c r="I94" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
+        <v>186</v>
+      </c>
+      <c r="F94" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>126</v>
       </c>
       <c r="B95" t="s">
         <v>127</v>
       </c>
-      <c r="H95" t="s">
-        <v>186</v>
-      </c>
-      <c r="I95" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
+        <v>186</v>
+      </c>
+      <c r="F95" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>123</v>
       </c>
       <c r="B96" t="s">
         <v>124</v>
       </c>
-      <c r="H96" t="s">
-        <v>186</v>
-      </c>
-      <c r="I96" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
+        <v>186</v>
+      </c>
+      <c r="F96" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>125</v>
       </c>
       <c r="B97" t="s">
         <v>128</v>
       </c>
-      <c r="H97" t="s">
-        <v>186</v>
-      </c>
-      <c r="I97" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
+        <v>186</v>
+      </c>
+      <c r="F97" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>129</v>
       </c>
       <c r="B98" t="s">
         <v>128</v>
       </c>
-      <c r="H98" t="s">
-        <v>186</v>
-      </c>
-      <c r="I98" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
+        <v>186</v>
+      </c>
+      <c r="F98" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>132</v>
       </c>
       <c r="B99" t="s">
         <v>133</v>
       </c>
-      <c r="H99" t="s">
-        <v>186</v>
-      </c>
-      <c r="I99" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
+        <v>186</v>
+      </c>
+      <c r="F99" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>132</v>
       </c>
       <c r="B100" t="s">
         <v>134</v>
       </c>
-      <c r="H100" t="s">
-        <v>186</v>
-      </c>
-      <c r="I100" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
+        <v>186</v>
+      </c>
+      <c r="F100" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>132</v>
       </c>
       <c r="B101" t="s">
         <v>135</v>
       </c>
-      <c r="H101" t="s">
-        <v>186</v>
-      </c>
-      <c r="I101" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
+        <v>186</v>
+      </c>
+      <c r="F101" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>132</v>
       </c>
       <c r="B102" t="s">
         <v>136</v>
       </c>
-      <c r="H102" t="s">
-        <v>186</v>
-      </c>
-      <c r="I102" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>186</v>
+      </c>
+      <c r="F102" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>132</v>
       </c>
       <c r="B103" t="s">
         <v>137</v>
       </c>
-      <c r="H103" t="s">
-        <v>186</v>
-      </c>
-      <c r="I103" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
+        <v>186</v>
+      </c>
+      <c r="F103" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>132</v>
       </c>
       <c r="B104" t="s">
         <v>138</v>
       </c>
-      <c r="H104" t="s">
-        <v>186</v>
-      </c>
-      <c r="I104" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>186</v>
+      </c>
+      <c r="F104" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>130</v>
       </c>
       <c r="B105" t="s">
         <v>131</v>
       </c>
-      <c r="H105" t="s">
-        <v>186</v>
-      </c>
-      <c r="I105" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
+        <v>186</v>
+      </c>
+      <c r="F105" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>144</v>
       </c>
       <c r="B106" t="s">
         <v>144</v>
       </c>
-      <c r="H106" t="s">
-        <v>186</v>
-      </c>
-      <c r="I106" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E106" t="s">
+        <v>186</v>
+      </c>
+      <c r="F106" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>139</v>
       </c>
       <c r="B107" t="s">
         <v>140</v>
       </c>
-      <c r="H107" t="s">
-        <v>186</v>
-      </c>
-      <c r="I107" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E107" t="s">
+        <v>186</v>
+      </c>
+      <c r="F107" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>141</v>
       </c>
       <c r="B108" t="s">
         <v>142</v>
       </c>
-      <c r="H108" t="s">
-        <v>186</v>
-      </c>
-      <c r="I108" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E108" t="s">
+        <v>186</v>
+      </c>
+      <c r="F108" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>143</v>
       </c>
       <c r="B109" t="s">
-        <v>208</v>
-      </c>
-      <c r="H109" t="s">
-        <v>186</v>
-      </c>
-      <c r="I109" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+      <c r="E109" t="s">
+        <v>186</v>
+      </c>
+      <c r="F109" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>160</v>
       </c>
@@ -2631,130 +2574,124 @@
       <c r="E110" t="s">
         <v>186</v>
       </c>
-      <c r="G110" t="s">
-        <v>186</v>
-      </c>
-      <c r="H110" t="s">
-        <v>186</v>
-      </c>
-      <c r="I110" t="s">
+      <c r="F110" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>160</v>
       </c>
       <c r="B111" t="s">
         <v>161</v>
       </c>
-      <c r="H111" t="s">
-        <v>186</v>
-      </c>
-      <c r="I111" t="s">
+      <c r="E111" t="s">
+        <v>186</v>
+      </c>
+      <c r="F111" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>145</v>
       </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
-      <c r="H112" t="s">
-        <v>186</v>
-      </c>
-      <c r="I112" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E112" t="s">
+        <v>186</v>
+      </c>
+      <c r="F112" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>147</v>
       </c>
       <c r="B113" t="s">
         <v>148</v>
       </c>
-      <c r="H113" t="s">
-        <v>186</v>
-      </c>
-      <c r="I113" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E113" t="s">
+        <v>186</v>
+      </c>
+      <c r="F113" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>192</v>
       </c>
       <c r="B114" t="s">
         <v>193</v>
       </c>
-      <c r="H114" t="s">
-        <v>186</v>
-      </c>
-      <c r="I114" t="s">
+      <c r="E114" t="s">
+        <v>186</v>
+      </c>
+      <c r="F114" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>149</v>
       </c>
       <c r="B115" t="s">
         <v>150</v>
       </c>
-      <c r="H115" t="s">
-        <v>186</v>
-      </c>
-      <c r="I115" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E115" t="s">
+        <v>186</v>
+      </c>
+      <c r="F115" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>151</v>
       </c>
       <c r="B116" t="s">
-        <v>209</v>
-      </c>
-      <c r="H116" t="s">
-        <v>186</v>
-      </c>
-      <c r="I116" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+      <c r="E116" t="s">
+        <v>186</v>
+      </c>
+      <c r="F116" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>168</v>
       </c>
       <c r="B117" t="s">
         <v>167</v>
       </c>
-      <c r="H117" t="s">
-        <v>186</v>
-      </c>
-      <c r="I117" t="s">
+      <c r="E117" t="s">
+        <v>186</v>
+      </c>
+      <c r="F117" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>152</v>
       </c>
       <c r="B118" t="s">
         <v>153</v>
       </c>
-      <c r="H118" t="s">
-        <v>186</v>
-      </c>
-      <c r="I118" t="s">
+      <c r="E118" t="s">
+        <v>186</v>
+      </c>
+      <c r="F118" t="s">
         <v>157</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I118"/>
+  <autoFilter ref="A1:F118"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2775,7 +2712,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>